<commit_message>
Try adding features to streamlit
interactive map and feature importance
</commit_message>
<xml_diff>
--- a/sample_input.xlsx
+++ b/sample_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChristopherTanMengHu\Desktop\streamlit-share-test\streamlit-share-webapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0385CFF4-9E01-40CA-AD23-F0E5EFE6F47A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7E6B3A-76AE-429F-A86F-EE7811543361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{7C23475E-A92A-480F-80E6-71B9D2FD9154}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{7C23475E-A92A-480F-80E6-71B9D2FD9154}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>incomeperperson</t>
   </si>
@@ -46,12 +46,18 @@
   <si>
     <t>urbanrate</t>
   </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +72,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -88,7 +100,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -96,6 +108,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,20 +443,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22935E44-89B5-40ED-B4EE-5B54162628B1}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="15.6328125" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,8 +466,14 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>25000</v>
       </c>
@@ -464,8 +483,14 @@
       <c r="C2" s="2">
         <v>75</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>1.4049400000000001</v>
+      </c>
+      <c r="E2">
+        <v>103.898037</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>32000</v>
       </c>
@@ -475,8 +500,14 @@
       <c r="C3" s="2">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>1.292109</v>
+      </c>
+      <c r="E3">
+        <v>103.80236499999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>15000</v>
       </c>
@@ -486,8 +517,136 @@
       <c r="C4" s="2">
         <v>60</v>
       </c>
+      <c r="D4" s="3">
+        <v>1.3344830000000001</v>
+      </c>
+      <c r="E4" s="3">
+        <v>103.91136400000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>20000</v>
+      </c>
+      <c r="B5" s="2">
+        <v>75</v>
+      </c>
+      <c r="C5" s="2">
+        <v>80</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1.3948799999999999</v>
+      </c>
+      <c r="E5" s="3">
+        <v>103.91258000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>50000</v>
+      </c>
+      <c r="B6" s="2">
+        <v>55</v>
+      </c>
+      <c r="C6" s="2">
+        <v>75</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.3992199999999999</v>
+      </c>
+      <c r="E6" s="3">
+        <v>103.908923</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>45000</v>
+      </c>
+      <c r="B7" s="2">
+        <v>67</v>
+      </c>
+      <c r="C7" s="2">
+        <v>56</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.3988560000000001</v>
+      </c>
+      <c r="E7" s="3">
+        <v>103.917197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>50000</v>
+      </c>
+      <c r="B8" s="2">
+        <v>89</v>
+      </c>
+      <c r="C8" s="2">
+        <v>74</v>
+      </c>
+      <c r="D8">
+        <v>1.451803</v>
+      </c>
+      <c r="E8">
+        <v>103.81670099999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>48000</v>
+      </c>
+      <c r="B9" s="2">
+        <v>59</v>
+      </c>
+      <c r="C9" s="2">
+        <v>56</v>
+      </c>
+      <c r="D9">
+        <v>1.4531909999999999</v>
+      </c>
+      <c r="E9">
+        <v>103.819068</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>61000</v>
+      </c>
+      <c r="B10" s="2">
+        <v>67</v>
+      </c>
+      <c r="C10" s="2">
+        <v>47</v>
+      </c>
+      <c r="D10">
+        <v>1.4543459999999999</v>
+      </c>
+      <c r="E10">
+        <v>103.81642600000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>12500</v>
+      </c>
+      <c r="B11">
+        <v>56</v>
+      </c>
+      <c r="C11" s="2">
+        <v>39</v>
+      </c>
+      <c r="D11">
+        <v>1.452736</v>
+      </c>
+      <c r="E11">
+        <v>103.817249</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Sensitive</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Corrected error in sample_input
swapped latitude and longitude labels
</commit_message>
<xml_diff>
--- a/sample_input.xlsx
+++ b/sample_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChristopherTanMengHu\Desktop\streamlit-share-test\streamlit-share-webapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7E6B3A-76AE-429F-A86F-EE7811543361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EDB7CB8-750D-44E0-89A7-BF0BFA9CD80A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{7C23475E-A92A-480F-80E6-71B9D2FD9154}"/>
+    <workbookView xWindow="5340" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{7C23475E-A92A-480F-80E6-71B9D2FD9154}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -446,7 +446,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -456,7 +456,7 @@
     <col min="3" max="3" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -467,10 +467,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>